<commit_message>
fixed issues with Danielle's submission
</commit_message>
<xml_diff>
--- a/data-raw/submissions/Danielle Kern - Thrones Pool.xlsx
+++ b/data-raw/submissions/Danielle Kern - Thrones Pool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tylerbradley/Documents/thrones-pool/data-raw/submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969EC0FB-D50A-8E44-BB80-1BF8618F7398}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76694821-CD2D-FE42-9BD9-8A1BB05BB105}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="61">
   <si>
     <t>Name:</t>
   </si>
@@ -182,9 +182,6 @@
   </si>
   <si>
     <t>Who kills Cercei? … if killed (3) **If you think this bitch lives pick her name**</t>
-  </si>
-  <si>
-    <t>Arya</t>
   </si>
   <si>
     <t>Will we see an undead Ned Stark? (2) … yes or no answer</t>
@@ -578,6 +575,13 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -594,13 +598,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -922,7 +919,7 @@
   <dimension ref="A2:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -943,12 +940,12 @@
     </row>
     <row r="3" spans="1:5" ht="17">
       <c r="A3" s="5"/>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="29"/>
     </row>
     <row r="4" spans="1:5" ht="15">
       <c r="A4" s="5"/>
@@ -973,7 +970,7 @@
       <c r="C5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="22" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="12" t="s">
@@ -1267,110 +1264,110 @@
     </row>
     <row r="25" spans="1:5" ht="17">
       <c r="A25" s="5"/>
-      <c r="B25" s="27" t="s">
+      <c r="B25" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
       <c r="E25" s="16" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1">
       <c r="A26" s="5"/>
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="22"/>
-      <c r="D26" s="23"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="26"/>
       <c r="E26" s="17" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1">
       <c r="A27" s="5"/>
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
       <c r="E27" s="17" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1">
       <c r="A28" s="5"/>
-      <c r="B28" s="29" t="s">
+      <c r="B28" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="C28" s="22"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="30" t="s">
+      <c r="C28" s="25"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="21" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1">
       <c r="A29" s="5"/>
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="C29" s="22"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="32" t="s">
+      <c r="C29" s="25"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="23" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1">
       <c r="A30" s="5"/>
-      <c r="B30" s="21" t="s">
+      <c r="B30" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="22"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="18" t="s">
-        <v>54</v>
+      <c r="C30" s="25"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="23" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1">
       <c r="A31" s="5"/>
-      <c r="B31" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="30" t="s">
-        <v>61</v>
+      <c r="B31" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="21" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1">
       <c r="A32" s="5"/>
-      <c r="B32" s="21" t="s">
+      <c r="B32" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="25"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="19" t="s">
         <v>56</v>
-      </c>
-      <c r="C32" s="22"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="19" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15.75" customHeight="1">
       <c r="A33" s="5"/>
-      <c r="B33" s="21" t="s">
+      <c r="B33" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="25"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="20" t="s">
         <v>58</v>
-      </c>
-      <c r="C33" s="22"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="20" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15.75" customHeight="1">
       <c r="A34" s="5"/>
-      <c r="B34" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="C34" s="22"/>
-      <c r="D34" s="23"/>
+      <c r="B34" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="25"/>
+      <c r="D34" s="26"/>
       <c r="E34" s="18" t="s">
         <v>26</v>
       </c>

</xml_diff>